<commit_message>
Updated some 3D models Updated BOM sheet Added bodge instructions Added some documentation
</commit_message>
<xml_diff>
--- a/Hardware/Final/DCZIA DC31 BADGE BOM.xlsx
+++ b/Hardware/Final/DCZIA DC31 BADGE BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hamster\Documents\Development\dczia\Defcon31-Badge\Hardware\Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263D53A5-8FF5-4FC0-92CD-F653CADE6F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F13DC4E-5EE9-4D30-9B1E-EE24D1443953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9864" yWindow="852" windowWidth="28872" windowHeight="17976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="62844" yWindow="9708" windowWidth="21540" windowHeight="14832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="162">
   <si>
     <t>Refdes</t>
   </si>
@@ -503,13 +503,16 @@
   </si>
   <si>
     <t>KYCON</t>
+  </si>
+  <si>
+    <t>Height</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -563,6 +566,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -585,7 +601,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -601,6 +617,9 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -885,11 +904,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:O983"/>
+  <dimension ref="A1:P983"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H44" sqref="H44"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -900,15 +919,16 @@
     <col min="4" max="4" width="18" style="6" customWidth="1"/>
     <col min="5" max="5" width="13.109375" customWidth="1"/>
     <col min="6" max="6" width="18.44140625" customWidth="1"/>
-    <col min="7" max="7" width="14.44140625" style="6"/>
-    <col min="8" max="8" width="14.6640625" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" customWidth="1"/>
-    <col min="11" max="11" width="8.44140625" customWidth="1"/>
-    <col min="12" max="12" width="10.44140625" customWidth="1"/>
-    <col min="13" max="13" width="12.88671875" customWidth="1"/>
+    <col min="7" max="7" width="7.77734375" style="15" customWidth="1"/>
+    <col min="8" max="8" width="8.5546875" style="6" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" customWidth="1"/>
+    <col min="12" max="12" width="8.44140625" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" customWidth="1"/>
+    <col min="14" max="14" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -927,43 +947,46 @@
       <c r="F1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>137</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>136</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>45</v>
       </c>
@@ -971,20 +994,22 @@
         <v>41</v>
       </c>
       <c r="D3" s="7"/>
-      <c r="G3" s="7"/>
-    </row>
-    <row r="4" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G3" s="15"/>
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D4" s="7"/>
-      <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G4" s="15"/>
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>155</v>
       </c>
@@ -1003,32 +1028,33 @@
       <c r="F6" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="1">
+      <c r="G6" s="16"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="1">
         <v>0.98199999999999998</v>
       </c>
-      <c r="I6" s="1">
+      <c r="J6" s="1">
         <v>5</v>
       </c>
-      <c r="J6" s="1">
-        <f>H6*I6</f>
+      <c r="K6" s="1">
+        <f>I6*J6</f>
         <v>4.91</v>
       </c>
-      <c r="K6" s="1">
-        <v>0</v>
-      </c>
       <c r="L6" s="1">
-        <f t="shared" ref="L6" si="0">IF((($N$2 * I6) - K6) &lt; 0, 0, (($N$2 * I6) - K6))</f>
+        <v>0</v>
+      </c>
+      <c r="M6" s="1">
+        <f t="shared" ref="M6" si="0">IF((($O$2 * J6) - L6) &lt; 0, 0, (($O$2 * J6) - L6))</f>
         <v>550</v>
       </c>
-      <c r="M6" s="1">
-        <f>L6*H6</f>
+      <c r="N6" s="1">
+        <f>M6*I6</f>
         <v>540.1</v>
       </c>
-      <c r="N6" s="1"/>
       <c r="O6" s="1"/>
-    </row>
-    <row r="7" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P6" s="1"/>
+    </row>
+    <row r="7" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>156</v>
       </c>
@@ -1047,33 +1073,34 @@
       <c r="F7" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="G7" s="7"/>
-      <c r="H7" s="1">
+      <c r="G7" s="16"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="1">
         <v>1.52536</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J7" s="1">
         <v>5</v>
       </c>
-      <c r="J7" s="1">
-        <f>H7*I7</f>
+      <c r="K7" s="1">
+        <f>I7*J7</f>
         <v>7.6268000000000002</v>
       </c>
-      <c r="K7" s="1">
-        <v>0</v>
-      </c>
       <c r="L7" s="1">
-        <f t="shared" ref="L7:L35" si="1">IF((($N$2 * I7) - K7) &lt; 0, 0, (($N$2 * I7) - K7))</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="1">
+        <f t="shared" ref="M7:M35" si="1">IF((($O$2 * J7) - L7) &lt; 0, 0, (($O$2 * J7) - L7))</f>
         <v>550</v>
       </c>
-      <c r="M7" s="1">
-        <f>L7*H7</f>
+      <c r="N7" s="1">
+        <f>M7*I7</f>
         <v>838.94799999999998</v>
       </c>
-      <c r="N7" s="1">
+      <c r="O7" s="1">
         <v>550</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>79</v>
       </c>
@@ -1092,33 +1119,36 @@
       <c r="F8" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="G8" s="7"/>
-      <c r="H8" s="1">
+      <c r="G8" s="16">
+        <v>1</v>
+      </c>
+      <c r="H8" s="7"/>
+      <c r="I8" s="1">
         <v>2.06</v>
       </c>
-      <c r="I8" s="1">
+      <c r="J8" s="1">
         <v>1</v>
       </c>
-      <c r="J8" s="1">
-        <f>H8*I8</f>
+      <c r="K8" s="1">
+        <f>I8*J8</f>
         <v>2.06</v>
       </c>
-      <c r="K8" s="1">
-        <v>0</v>
-      </c>
       <c r="L8" s="1">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="M8" s="1">
-        <f t="shared" ref="M8:M35" si="2">L8*H8</f>
+      <c r="N8" s="1">
+        <f t="shared" ref="N8:N35" si="2">M8*I8</f>
         <v>226.6</v>
       </c>
-      <c r="N8" s="1">
+      <c r="O8" s="1">
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
@@ -1137,33 +1167,34 @@
       <c r="F9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="1">
+      <c r="G9" s="16"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="1">
         <v>0.47699999999999998</v>
       </c>
-      <c r="I9" s="1">
+      <c r="J9" s="1">
         <v>1</v>
       </c>
-      <c r="J9" s="1">
-        <f t="shared" ref="J9:J47" si="3">H9*I9</f>
+      <c r="K9" s="1">
+        <f t="shared" ref="K9:K47" si="3">I9*J9</f>
         <v>0.47699999999999998</v>
       </c>
-      <c r="K9" s="1">
-        <v>0</v>
-      </c>
       <c r="L9" s="1">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="M9" s="1">
+      <c r="N9" s="1">
         <f t="shared" si="2"/>
         <v>52.47</v>
       </c>
-      <c r="N9" s="1">
+      <c r="O9" s="1">
         <v>110</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>76</v>
       </c>
@@ -1182,33 +1213,36 @@
       <c r="F10" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="7"/>
-      <c r="H10" s="1">
+      <c r="G10" s="16">
+        <v>1</v>
+      </c>
+      <c r="H10" s="7"/>
+      <c r="I10" s="1">
         <v>0.18</v>
       </c>
-      <c r="I10" s="1">
+      <c r="J10" s="1">
         <v>1</v>
       </c>
-      <c r="J10" s="1">
+      <c r="K10" s="1">
         <f t="shared" si="3"/>
         <v>0.18</v>
       </c>
-      <c r="K10" s="1">
+      <c r="L10" s="1">
         <v>100</v>
       </c>
-      <c r="L10" s="1">
+      <c r="M10" s="1">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="M10" s="1">
+      <c r="N10" s="1">
         <f t="shared" si="2"/>
         <v>1.7999999999999998</v>
       </c>
-      <c r="N10" s="1">
+      <c r="O10" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>74</v>
       </c>
@@ -1227,33 +1261,34 @@
       <c r="F11" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="1">
+      <c r="G11" s="15"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="1">
         <v>6</v>
       </c>
-      <c r="I11" s="1">
+      <c r="J11" s="1">
         <v>1</v>
       </c>
-      <c r="J11" s="1">
+      <c r="K11" s="1">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="K11" s="1">
-        <v>0</v>
-      </c>
       <c r="L11" s="1">
+        <v>0</v>
+      </c>
+      <c r="M11" s="1">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="M11" s="1">
+      <c r="N11" s="1">
         <f t="shared" si="2"/>
         <v>660</v>
       </c>
-      <c r="N11" s="1">
+      <c r="O11" s="1">
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>75</v>
       </c>
@@ -1272,33 +1307,36 @@
       <c r="F12" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="1">
+      <c r="G12" s="16">
+        <v>1</v>
+      </c>
+      <c r="H12" s="7"/>
+      <c r="I12" s="1">
         <v>2.11</v>
       </c>
-      <c r="I12" s="1">
+      <c r="J12" s="1">
         <v>1</v>
       </c>
-      <c r="J12" s="1">
+      <c r="K12" s="1">
         <f t="shared" si="3"/>
         <v>2.11</v>
       </c>
-      <c r="K12" s="1">
-        <v>0</v>
-      </c>
       <c r="L12" s="1">
+        <v>0</v>
+      </c>
+      <c r="M12" s="1">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="M12" s="1">
+      <c r="N12" s="1">
         <f t="shared" si="2"/>
         <v>232.1</v>
       </c>
-      <c r="N12" s="1">
+      <c r="O12" s="1">
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>77</v>
       </c>
@@ -1317,33 +1355,36 @@
       <c r="F13" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="1">
+      <c r="G13" s="15">
+        <v>1</v>
+      </c>
+      <c r="H13" s="7"/>
+      <c r="I13" s="1">
         <v>1.03</v>
       </c>
-      <c r="I13" s="1">
+      <c r="J13" s="1">
         <v>1</v>
       </c>
-      <c r="J13" s="1">
+      <c r="K13" s="1">
         <f t="shared" si="3"/>
         <v>1.03</v>
       </c>
-      <c r="K13" s="1">
-        <v>0</v>
-      </c>
       <c r="L13" s="1">
+        <v>0</v>
+      </c>
+      <c r="M13" s="1">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="M13" s="1">
+      <c r="N13" s="1">
         <f t="shared" si="2"/>
         <v>113.3</v>
       </c>
-      <c r="N13" s="1">
+      <c r="O13" s="1">
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>46</v>
       </c>
@@ -1356,30 +1397,31 @@
       <c r="D14" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G14" s="7"/>
-      <c r="H14" s="1">
+      <c r="G14" s="15"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="1">
         <v>0.08</v>
       </c>
-      <c r="I14" s="1">
+      <c r="J14" s="1">
         <v>1</v>
       </c>
-      <c r="J14" s="1">
+      <c r="K14" s="1">
         <f t="shared" si="3"/>
         <v>0.08</v>
       </c>
-      <c r="K14" s="1">
+      <c r="L14" s="1">
         <v>110</v>
       </c>
-      <c r="L14" s="1">
+      <c r="M14" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M14" s="1">
+      <c r="N14" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>84</v>
       </c>
@@ -1392,30 +1434,31 @@
       <c r="D15" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="G15" s="7"/>
-      <c r="H15" s="1">
+      <c r="G15" s="15"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="1">
         <v>0.05</v>
       </c>
-      <c r="I15" s="1">
+      <c r="J15" s="1">
         <v>10</v>
       </c>
-      <c r="J15" s="1">
+      <c r="K15" s="1">
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K15" s="1">
+      <c r="L15" s="1">
         <v>1500</v>
       </c>
-      <c r="L15" s="1">
+      <c r="M15" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M15" s="1">
+      <c r="N15" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>32</v>
       </c>
@@ -1425,30 +1468,31 @@
       <c r="D16" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="G16" s="7"/>
-      <c r="H16" s="1">
+      <c r="G16" s="15"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="1">
         <v>0.6</v>
       </c>
-      <c r="I16" s="1">
+      <c r="J16" s="1">
         <v>1</v>
       </c>
-      <c r="J16" s="1">
+      <c r="K16" s="1">
         <f t="shared" si="3"/>
         <v>0.6</v>
       </c>
-      <c r="K16" s="1">
+      <c r="L16" s="1">
         <v>110</v>
       </c>
-      <c r="L16" s="1">
+      <c r="M16" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M16" s="1">
+      <c r="N16" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>10</v>
       </c>
@@ -1458,30 +1502,31 @@
       <c r="D17" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="G17" s="7"/>
-      <c r="H17" s="1">
+      <c r="G17" s="15"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="1">
         <v>1.85</v>
       </c>
-      <c r="I17" s="1">
+      <c r="J17" s="1">
         <v>1</v>
       </c>
-      <c r="J17" s="1">
+      <c r="K17" s="1">
         <f t="shared" si="3"/>
         <v>1.85</v>
       </c>
-      <c r="K17" s="1">
+      <c r="L17" s="1">
         <v>110</v>
       </c>
-      <c r="L17" s="1">
+      <c r="M17" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M17" s="1">
+      <c r="N17" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>114</v>
       </c>
@@ -1497,35 +1542,38 @@
       <c r="F18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="G18" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="H18" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="H18" s="1">
+      <c r="I18" s="1">
         <v>0.127</v>
       </c>
-      <c r="I18" s="1">
+      <c r="J18" s="1">
         <v>16</v>
       </c>
-      <c r="J18" s="1">
+      <c r="K18" s="1">
         <f t="shared" si="3"/>
         <v>2.032</v>
       </c>
-      <c r="K18" s="1">
-        <v>0</v>
-      </c>
       <c r="L18" s="1">
+        <v>0</v>
+      </c>
+      <c r="M18" s="1">
         <f t="shared" si="1"/>
         <v>1760</v>
       </c>
-      <c r="M18" s="1">
+      <c r="N18" s="1">
         <f t="shared" si="2"/>
         <v>223.52</v>
       </c>
-      <c r="N18" s="1">
+      <c r="O18" s="1">
         <v>2500</v>
       </c>
     </row>
-    <row r="19" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>42</v>
       </c>
@@ -1541,32 +1589,35 @@
       <c r="F19" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="G19" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="H19" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="H19" s="1">
+      <c r="I19" s="1">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="I19" s="1">
+      <c r="J19" s="1">
         <v>4</v>
       </c>
-      <c r="J19" s="1">
+      <c r="K19" s="1">
         <f t="shared" si="3"/>
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="K19" s="1">
+      <c r="L19" s="1">
         <v>1000</v>
       </c>
-      <c r="L19" s="1">
+      <c r="M19" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M19" s="1">
+      <c r="N19" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>43</v>
       </c>
@@ -1582,35 +1633,38 @@
       <c r="F20" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="G20" s="15">
+        <v>1.45</v>
+      </c>
+      <c r="H20" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="H20" s="1">
+      <c r="I20" s="1">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="I20" s="1">
+      <c r="J20" s="1">
         <v>1</v>
       </c>
-      <c r="J20" s="1">
+      <c r="K20" s="1">
         <f t="shared" si="3"/>
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="K20" s="1">
-        <v>0</v>
-      </c>
       <c r="L20" s="1">
+        <v>0</v>
+      </c>
+      <c r="M20" s="1">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="M20" s="1">
+      <c r="N20" s="1">
         <f t="shared" si="2"/>
         <v>3.74</v>
       </c>
-      <c r="N20" s="1">
+      <c r="O20" s="1">
         <v>125</v>
       </c>
     </row>
-    <row r="21" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>44</v>
       </c>
@@ -1626,35 +1680,38 @@
       <c r="F21" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="G21" s="7" t="s">
+      <c r="G21" s="15">
+        <v>1.45</v>
+      </c>
+      <c r="H21" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="H21" s="1">
+      <c r="I21" s="1">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="I21" s="1">
+      <c r="J21" s="1">
         <v>1</v>
       </c>
-      <c r="J21" s="1">
+      <c r="K21" s="1">
         <f t="shared" si="3"/>
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="K21" s="1">
-        <v>0</v>
-      </c>
       <c r="L21" s="1">
+        <v>0</v>
+      </c>
+      <c r="M21" s="1">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="M21" s="1">
+      <c r="N21" s="1">
         <f t="shared" si="2"/>
         <v>3.8500000000000005</v>
       </c>
-      <c r="N21" s="1">
+      <c r="O21" s="1">
         <v>125</v>
       </c>
     </row>
-    <row r="22" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>127</v>
       </c>
@@ -1670,35 +1727,38 @@
       <c r="F22" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="G22" s="15">
+        <v>1.45</v>
+      </c>
+      <c r="H22" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="H22" s="1">
+      <c r="I22" s="1">
         <v>3.1E-2</v>
       </c>
-      <c r="I22" s="1">
+      <c r="J22" s="1">
         <v>1</v>
       </c>
-      <c r="J22" s="1">
+      <c r="K22" s="1">
         <f t="shared" si="3"/>
         <v>3.1E-2</v>
       </c>
-      <c r="K22" s="1">
-        <v>0</v>
-      </c>
       <c r="L22" s="1">
+        <v>0</v>
+      </c>
+      <c r="M22" s="1">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="M22" s="1">
+      <c r="N22" s="1">
         <f t="shared" si="2"/>
         <v>3.41</v>
       </c>
-      <c r="N22" s="1">
+      <c r="O22" s="1">
         <v>125</v>
       </c>
     </row>
-    <row r="23" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>49</v>
       </c>
@@ -1714,35 +1774,36 @@
       <c r="F23" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="G23" s="7" t="s">
+      <c r="G23" s="15"/>
+      <c r="H23" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="H23" s="1">
+      <c r="I23" s="1">
         <v>0.16700000000000001</v>
       </c>
-      <c r="I23" s="1">
+      <c r="J23" s="1">
         <v>1</v>
       </c>
-      <c r="J23" s="1">
+      <c r="K23" s="1">
         <f t="shared" si="3"/>
         <v>0.16700000000000001</v>
       </c>
-      <c r="K23" s="1">
-        <v>0</v>
-      </c>
       <c r="L23" s="1">
+        <v>0</v>
+      </c>
+      <c r="M23" s="1">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="M23" s="1">
+      <c r="N23" s="1">
         <f t="shared" si="2"/>
         <v>18.37</v>
       </c>
-      <c r="N23" s="1">
+      <c r="O23" s="1">
         <v>125</v>
       </c>
     </row>
-    <row r="24" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>51</v>
       </c>
@@ -1758,35 +1819,38 @@
       <c r="F24" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="G24" s="7" t="s">
+      <c r="G24" s="15">
+        <v>1</v>
+      </c>
+      <c r="H24" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="H24" s="1">
+      <c r="I24" s="1">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="I24" s="1">
+      <c r="J24" s="1">
         <v>1</v>
       </c>
-      <c r="J24" s="1">
+      <c r="K24" s="1">
         <f t="shared" si="3"/>
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="K24" s="1">
+      <c r="L24" s="1">
         <v>100</v>
       </c>
-      <c r="L24" s="1">
+      <c r="M24" s="1">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="M24" s="1">
+      <c r="N24" s="1">
         <f t="shared" si="2"/>
         <v>0.48</v>
       </c>
-      <c r="N24" s="1">
+      <c r="O24" s="1">
         <v>125</v>
       </c>
     </row>
-    <row r="25" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>54</v>
       </c>
@@ -1802,32 +1866,35 @@
       <c r="F25" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="G25" s="7" t="s">
+      <c r="G25" s="16">
+        <v>0.45</v>
+      </c>
+      <c r="H25" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="H25" s="1">
+      <c r="I25" s="1">
         <v>1E-3</v>
       </c>
-      <c r="I25" s="1">
+      <c r="J25" s="1">
         <v>2</v>
       </c>
-      <c r="J25" s="1">
+      <c r="K25" s="1">
         <f t="shared" si="3"/>
         <v>2E-3</v>
       </c>
-      <c r="K25" s="1">
+      <c r="L25" s="1">
         <v>5000</v>
       </c>
-      <c r="L25" s="1">
+      <c r="M25" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M25" s="1">
+      <c r="N25" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>56</v>
       </c>
@@ -1843,32 +1910,35 @@
       <c r="F26" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="G26" s="7" t="s">
+      <c r="G26" s="16">
+        <v>0.45</v>
+      </c>
+      <c r="H26" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="H26" s="1">
+      <c r="I26" s="1">
         <v>1E-3</v>
       </c>
-      <c r="I26" s="1">
+      <c r="J26" s="1">
         <v>1</v>
       </c>
-      <c r="J26" s="1">
+      <c r="K26" s="1">
         <f t="shared" si="3"/>
         <v>1E-3</v>
       </c>
-      <c r="K26" s="1">
+      <c r="L26" s="1">
         <v>5000</v>
       </c>
-      <c r="L26" s="1">
+      <c r="M26" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M26" s="1">
+      <c r="N26" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>58</v>
       </c>
@@ -1884,32 +1954,35 @@
       <c r="F27" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="G27" s="7" t="s">
+      <c r="G27" s="16">
+        <v>0.45</v>
+      </c>
+      <c r="H27" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="H27" s="1">
+      <c r="I27" s="1">
         <v>1E-3</v>
       </c>
-      <c r="I27" s="1">
+      <c r="J27" s="1">
         <v>3</v>
       </c>
-      <c r="J27" s="1">
+      <c r="K27" s="1">
         <f t="shared" si="3"/>
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="K27" s="1">
+      <c r="L27" s="1">
         <v>5000</v>
       </c>
-      <c r="L27" s="1">
+      <c r="M27" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M27" s="1">
+      <c r="N27" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>60</v>
       </c>
@@ -1925,32 +1998,35 @@
       <c r="F28" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="G28" s="7" t="s">
+      <c r="G28" s="16">
+        <v>0.45</v>
+      </c>
+      <c r="H28" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="H28" s="1">
+      <c r="I28" s="1">
         <v>1E-3</v>
       </c>
-      <c r="I28" s="1">
+      <c r="J28" s="1">
         <v>1</v>
       </c>
-      <c r="J28" s="1">
+      <c r="K28" s="1">
         <f t="shared" si="3"/>
         <v>1E-3</v>
       </c>
-      <c r="K28" s="1">
+      <c r="L28" s="1">
         <v>5000</v>
       </c>
-      <c r="L28" s="1">
+      <c r="M28" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M28" s="1">
+      <c r="N28" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>62</v>
       </c>
@@ -1966,32 +2042,35 @@
       <c r="F29" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="G29" s="7" t="s">
+      <c r="G29" s="16">
+        <v>0.45</v>
+      </c>
+      <c r="H29" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="H29" s="1">
+      <c r="I29" s="1">
         <v>1E-3</v>
       </c>
-      <c r="I29" s="1">
+      <c r="J29" s="1">
         <v>1</v>
       </c>
-      <c r="J29" s="1">
+      <c r="K29" s="1">
         <f t="shared" si="3"/>
         <v>1E-3</v>
       </c>
-      <c r="K29" s="1">
+      <c r="L29" s="1">
         <v>5000</v>
       </c>
-      <c r="L29" s="1">
+      <c r="M29" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M29" s="1">
+      <c r="N29" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>64</v>
       </c>
@@ -2007,35 +2086,38 @@
       <c r="F30" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="G30" s="7" t="s">
+      <c r="G30" s="16">
+        <v>0.45</v>
+      </c>
+      <c r="H30" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="H30" s="1">
+      <c r="I30" s="1">
         <v>1E-3</v>
       </c>
-      <c r="I30" s="1">
+      <c r="J30" s="1">
         <v>1</v>
       </c>
-      <c r="J30" s="1">
+      <c r="K30" s="1">
         <f t="shared" si="3"/>
         <v>1E-3</v>
       </c>
-      <c r="K30" s="1">
-        <v>0</v>
-      </c>
       <c r="L30" s="1">
+        <v>0</v>
+      </c>
+      <c r="M30" s="1">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="M30" s="1">
+      <c r="N30" s="1">
         <f t="shared" si="2"/>
         <v>0.11</v>
       </c>
-      <c r="N30" s="1">
+      <c r="O30" s="1">
         <v>5000</v>
       </c>
     </row>
-    <row r="31" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>66</v>
       </c>
@@ -2051,35 +2133,38 @@
       <c r="F31" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="G31" s="7" t="s">
+      <c r="G31" s="16">
+        <v>0.45</v>
+      </c>
+      <c r="H31" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="H31" s="1">
+      <c r="I31" s="1">
         <v>1E-3</v>
       </c>
-      <c r="I31" s="1">
+      <c r="J31" s="1">
         <v>1</v>
       </c>
-      <c r="J31" s="1">
+      <c r="K31" s="1">
         <f t="shared" si="3"/>
         <v>1E-3</v>
       </c>
-      <c r="K31" s="1">
-        <v>0</v>
-      </c>
       <c r="L31" s="1">
+        <v>0</v>
+      </c>
+      <c r="M31" s="1">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="M31" s="1">
+      <c r="N31" s="1">
         <f t="shared" si="2"/>
         <v>0.11</v>
       </c>
-      <c r="N31" s="1">
+      <c r="O31" s="1">
         <v>5000</v>
       </c>
     </row>
-    <row r="32" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>68</v>
       </c>
@@ -2087,32 +2172,35 @@
         <v>69</v>
       </c>
       <c r="D32" s="7"/>
-      <c r="G32" s="7" t="s">
+      <c r="G32" s="16">
+        <v>0.45</v>
+      </c>
+      <c r="H32" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="H32" s="1">
+      <c r="I32" s="1">
         <v>1E-3</v>
       </c>
-      <c r="I32" s="1">
+      <c r="J32" s="1">
         <v>1</v>
       </c>
-      <c r="J32" s="1">
+      <c r="K32" s="1">
         <f t="shared" si="3"/>
         <v>1E-3</v>
       </c>
-      <c r="K32" s="1">
+      <c r="L32" s="1">
         <v>5000</v>
       </c>
-      <c r="L32" s="1">
+      <c r="M32" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M32" s="1">
+      <c r="N32" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>70</v>
       </c>
@@ -2120,30 +2208,31 @@
         <v>71</v>
       </c>
       <c r="D33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="1">
+      <c r="G33" s="15"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="1">
         <v>0.27</v>
       </c>
-      <c r="I33" s="1">
+      <c r="J33" s="1">
         <v>10</v>
       </c>
-      <c r="J33" s="1">
+      <c r="K33" s="1">
         <f t="shared" si="3"/>
         <v>2.7</v>
       </c>
-      <c r="K33" s="1">
+      <c r="L33" s="1">
         <v>1300</v>
       </c>
-      <c r="L33" s="1">
+      <c r="M33" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M33" s="1">
+      <c r="N33" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>72</v>
       </c>
@@ -2159,33 +2248,34 @@
       <c r="F34" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="G34" s="7"/>
-      <c r="H34" s="1">
+      <c r="G34" s="15"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="1">
         <v>1.1000000000000001</v>
       </c>
-      <c r="I34" s="1">
+      <c r="J34" s="1">
         <v>2</v>
       </c>
-      <c r="J34" s="1">
+      <c r="K34" s="1">
         <f t="shared" si="3"/>
         <v>2.2000000000000002</v>
       </c>
-      <c r="K34" s="1">
-        <v>0</v>
-      </c>
       <c r="L34" s="1">
+        <v>0</v>
+      </c>
+      <c r="M34" s="1">
         <f t="shared" si="1"/>
         <v>220</v>
       </c>
-      <c r="M34" s="1">
+      <c r="N34" s="1">
         <f t="shared" si="2"/>
         <v>242.00000000000003</v>
       </c>
-      <c r="N34" s="1">
+      <c r="O34" s="1">
         <v>125</v>
       </c>
     </row>
-    <row r="35" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>112</v>
       </c>
@@ -2201,52 +2291,55 @@
       <c r="F35" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="G35" s="7"/>
-      <c r="H35" s="1">
+      <c r="G35" s="15"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="1">
         <v>0.53400000000000003</v>
       </c>
-      <c r="I35" s="1">
+      <c r="J35" s="1">
         <v>1</v>
       </c>
-      <c r="J35" s="1">
+      <c r="K35" s="1">
         <f t="shared" si="3"/>
         <v>0.53400000000000003</v>
       </c>
-      <c r="K35" s="1">
-        <v>0</v>
-      </c>
       <c r="L35" s="1">
+        <v>0</v>
+      </c>
+      <c r="M35" s="1">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="M35" s="1">
+      <c r="N35" s="1">
         <f t="shared" si="2"/>
         <v>58.74</v>
       </c>
-      <c r="N35" s="1">
+      <c r="O35" s="1">
         <v>125</v>
       </c>
     </row>
-    <row r="36" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="J36" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="G36" s="15"/>
+      <c r="H36" s="7"/>
+      <c r="K36" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>105</v>
       </c>
       <c r="D37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="J37" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="G37" s="15"/>
+      <c r="H37" s="7"/>
+      <c r="K37" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="1" t="s">
         <v>106</v>
@@ -2255,19 +2348,20 @@
         <v>139</v>
       </c>
       <c r="D38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="1">
-        <v>1</v>
-      </c>
+      <c r="G38" s="15"/>
+      <c r="H38" s="7"/>
       <c r="I38" s="1">
         <v>1</v>
       </c>
       <c r="J38" s="1">
-        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="K38" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="1" t="s">
         <v>107</v>
@@ -2276,19 +2370,20 @@
         <v>140</v>
       </c>
       <c r="D39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="1">
+      <c r="G39" s="15"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="1">
         <v>2</v>
       </c>
-      <c r="I39" s="1">
+      <c r="J39" s="1">
         <v>1</v>
       </c>
-      <c r="J39" s="1">
+      <c r="K39" s="1">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="1" t="s">
         <v>108</v>
@@ -2297,19 +2392,20 @@
         <v>141</v>
       </c>
       <c r="D40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="1">
+      <c r="G40" s="15"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="1">
         <v>0.31</v>
       </c>
-      <c r="I40" s="1">
+      <c r="J40" s="1">
         <v>3</v>
       </c>
-      <c r="J40" s="1">
+      <c r="K40" s="1">
         <f t="shared" si="3"/>
         <v>0.92999999999999994</v>
       </c>
     </row>
-    <row r="41" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="1" t="s">
         <v>109</v>
@@ -2318,19 +2414,20 @@
         <v>141</v>
       </c>
       <c r="D41" s="7"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="1">
+      <c r="G41" s="15"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="1">
         <v>0.45</v>
       </c>
-      <c r="I41" s="1">
+      <c r="J41" s="1">
         <v>1</v>
       </c>
-      <c r="J41" s="1">
+      <c r="K41" s="1">
         <f t="shared" si="3"/>
         <v>0.45</v>
       </c>
     </row>
-    <row r="42" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="1" t="s">
         <v>110</v>
@@ -2339,19 +2436,20 @@
         <v>141</v>
       </c>
       <c r="D42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="1">
+      <c r="G42" s="15"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="1">
         <v>0.5</v>
       </c>
-      <c r="I42" s="1">
+      <c r="J42" s="1">
         <v>2</v>
       </c>
-      <c r="J42" s="1">
+      <c r="K42" s="1">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="1" t="s">
         <v>111</v>
@@ -2360,19 +2458,20 @@
         <v>141</v>
       </c>
       <c r="D43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="1">
+      <c r="G43" s="15"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="1">
         <v>0.25</v>
       </c>
-      <c r="I43" s="1">
+      <c r="J43" s="1">
         <v>10</v>
       </c>
-      <c r="J43" s="1">
+      <c r="K43" s="1">
         <f t="shared" si="3"/>
         <v>2.5</v>
       </c>
     </row>
-    <row r="44" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="1" t="s">
         <v>118</v>
@@ -2381,19 +2480,20 @@
         <v>141</v>
       </c>
       <c r="D44" s="7"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="1">
+      <c r="G44" s="15"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="1">
         <v>4</v>
       </c>
-      <c r="I44" s="1">
+      <c r="J44" s="1">
         <v>2</v>
       </c>
-      <c r="J44" s="1">
+      <c r="K44" s="1">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="1" t="s">
         <v>119</v>
@@ -2402,19 +2502,20 @@
         <v>142</v>
       </c>
       <c r="D45" s="7"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="1">
+      <c r="G45" s="15"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="1">
         <v>8</v>
       </c>
-      <c r="I45" s="1">
+      <c r="J45" s="1">
         <v>0.1</v>
       </c>
-      <c r="J45" s="1">
+      <c r="K45" s="1">
         <f t="shared" si="3"/>
         <v>0.8</v>
       </c>
     </row>
-    <row r="46" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="1" t="s">
         <v>120</v>
@@ -2423,80 +2524,84 @@
         <v>142</v>
       </c>
       <c r="D46" s="7"/>
-      <c r="G46" s="7"/>
-      <c r="H46" s="1">
+      <c r="G46" s="15"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="1">
         <v>0.25</v>
       </c>
-      <c r="I46" s="1">
+      <c r="J46" s="1">
         <v>1</v>
       </c>
-      <c r="J46" s="1">
+      <c r="K46" s="1">
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
     </row>
-    <row r="47" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D47" s="7"/>
-      <c r="G47" s="7"/>
-      <c r="J47" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="G47" s="15"/>
+      <c r="H47" s="7"/>
+      <c r="K47" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D48" s="8"/>
-      <c r="G48" s="8"/>
-    </row>
-    <row r="49" spans="2:8" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="G48" s="17"/>
+      <c r="H48" s="8"/>
+    </row>
+    <row r="49" spans="2:9" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
         <v>143</v>
       </c>
       <c r="D49" s="7"/>
-      <c r="G49" s="7"/>
-    </row>
-    <row r="50" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="G49" s="15"/>
+      <c r="H49" s="7"/>
+    </row>
+    <row r="50" spans="2:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
         <v>144</v>
       </c>
       <c r="C50">
         <v>2500</v>
       </c>
-      <c r="G50" s="9" t="s">
+      <c r="H50" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="H50">
-        <f>SUM(J2:J49)</f>
+      <c r="I50">
+        <f>SUM(K2:K49)</f>
         <v>52.189800000000005</v>
       </c>
     </row>
-    <row r="51" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
         <v>154</v>
       </c>
       <c r="C51">
         <v>1100</v>
       </c>
-      <c r="G51" s="6" t="s">
+      <c r="H51" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="H51">
-        <f>SUM(M7:M35)</f>
+      <c r="I51">
+        <f>SUM(N7:N35)</f>
         <v>2679.5479999999993</v>
       </c>
     </row>
-    <row r="52" spans="2:8" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="2:8" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="2:8" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="2:8" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="2:8" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="2:8" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="2:8" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="2:8" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="2:8" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="2:8" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="2:8" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="2:8" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="2:8" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="2:9" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="2:9" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="2:9" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="2:9" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="2:9" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="2:9" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="2:9" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="2:9" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="2:9" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="2:9" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="2:9" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="2:9" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="2:9" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="65" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="66" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="67" ht="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Various hardware changes (#44)
Updated some 3D models
Updated BOM sheet
Added bodge instructions
Added some documentation
</commit_message>
<xml_diff>
--- a/Hardware/Final/DCZIA DC31 BADGE BOM.xlsx
+++ b/Hardware/Final/DCZIA DC31 BADGE BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hamster\Documents\Development\dczia\Defcon31-Badge\Hardware\Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263D53A5-8FF5-4FC0-92CD-F653CADE6F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F13DC4E-5EE9-4D30-9B1E-EE24D1443953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9864" yWindow="852" windowWidth="28872" windowHeight="17976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="62844" yWindow="9708" windowWidth="21540" windowHeight="14832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="162">
   <si>
     <t>Refdes</t>
   </si>
@@ -503,13 +503,16 @@
   </si>
   <si>
     <t>KYCON</t>
+  </si>
+  <si>
+    <t>Height</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -563,6 +566,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -585,7 +601,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -601,6 +617,9 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -885,11 +904,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:O983"/>
+  <dimension ref="A1:P983"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H44" sqref="H44"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -900,15 +919,16 @@
     <col min="4" max="4" width="18" style="6" customWidth="1"/>
     <col min="5" max="5" width="13.109375" customWidth="1"/>
     <col min="6" max="6" width="18.44140625" customWidth="1"/>
-    <col min="7" max="7" width="14.44140625" style="6"/>
-    <col min="8" max="8" width="14.6640625" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" customWidth="1"/>
-    <col min="11" max="11" width="8.44140625" customWidth="1"/>
-    <col min="12" max="12" width="10.44140625" customWidth="1"/>
-    <col min="13" max="13" width="12.88671875" customWidth="1"/>
+    <col min="7" max="7" width="7.77734375" style="15" customWidth="1"/>
+    <col min="8" max="8" width="8.5546875" style="6" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" customWidth="1"/>
+    <col min="12" max="12" width="8.44140625" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" customWidth="1"/>
+    <col min="14" max="14" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -927,43 +947,46 @@
       <c r="F1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>137</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>136</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>45</v>
       </c>
@@ -971,20 +994,22 @@
         <v>41</v>
       </c>
       <c r="D3" s="7"/>
-      <c r="G3" s="7"/>
-    </row>
-    <row r="4" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G3" s="15"/>
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D4" s="7"/>
-      <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G4" s="15"/>
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>155</v>
       </c>
@@ -1003,32 +1028,33 @@
       <c r="F6" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="1">
+      <c r="G6" s="16"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="1">
         <v>0.98199999999999998</v>
       </c>
-      <c r="I6" s="1">
+      <c r="J6" s="1">
         <v>5</v>
       </c>
-      <c r="J6" s="1">
-        <f>H6*I6</f>
+      <c r="K6" s="1">
+        <f>I6*J6</f>
         <v>4.91</v>
       </c>
-      <c r="K6" s="1">
-        <v>0</v>
-      </c>
       <c r="L6" s="1">
-        <f t="shared" ref="L6" si="0">IF((($N$2 * I6) - K6) &lt; 0, 0, (($N$2 * I6) - K6))</f>
+        <v>0</v>
+      </c>
+      <c r="M6" s="1">
+        <f t="shared" ref="M6" si="0">IF((($O$2 * J6) - L6) &lt; 0, 0, (($O$2 * J6) - L6))</f>
         <v>550</v>
       </c>
-      <c r="M6" s="1">
-        <f>L6*H6</f>
+      <c r="N6" s="1">
+        <f>M6*I6</f>
         <v>540.1</v>
       </c>
-      <c r="N6" s="1"/>
       <c r="O6" s="1"/>
-    </row>
-    <row r="7" spans="1:15" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P6" s="1"/>
+    </row>
+    <row r="7" spans="1:16" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>156</v>
       </c>
@@ -1047,33 +1073,34 @@
       <c r="F7" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="G7" s="7"/>
-      <c r="H7" s="1">
+      <c r="G7" s="16"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="1">
         <v>1.52536</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J7" s="1">
         <v>5</v>
       </c>
-      <c r="J7" s="1">
-        <f>H7*I7</f>
+      <c r="K7" s="1">
+        <f>I7*J7</f>
         <v>7.6268000000000002</v>
       </c>
-      <c r="K7" s="1">
-        <v>0</v>
-      </c>
       <c r="L7" s="1">
-        <f t="shared" ref="L7:L35" si="1">IF((($N$2 * I7) - K7) &lt; 0, 0, (($N$2 * I7) - K7))</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="1">
+        <f t="shared" ref="M7:M35" si="1">IF((($O$2 * J7) - L7) &lt; 0, 0, (($O$2 * J7) - L7))</f>
         <v>550</v>
       </c>
-      <c r="M7" s="1">
-        <f>L7*H7</f>
+      <c r="N7" s="1">
+        <f>M7*I7</f>
         <v>838.94799999999998</v>
       </c>
-      <c r="N7" s="1">
+      <c r="O7" s="1">
         <v>550</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>79</v>
       </c>
@@ -1092,33 +1119,36 @@
       <c r="F8" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="G8" s="7"/>
-      <c r="H8" s="1">
+      <c r="G8" s="16">
+        <v>1</v>
+      </c>
+      <c r="H8" s="7"/>
+      <c r="I8" s="1">
         <v>2.06</v>
       </c>
-      <c r="I8" s="1">
+      <c r="J8" s="1">
         <v>1</v>
       </c>
-      <c r="J8" s="1">
-        <f>H8*I8</f>
+      <c r="K8" s="1">
+        <f>I8*J8</f>
         <v>2.06</v>
       </c>
-      <c r="K8" s="1">
-        <v>0</v>
-      </c>
       <c r="L8" s="1">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="M8" s="1">
-        <f t="shared" ref="M8:M35" si="2">L8*H8</f>
+      <c r="N8" s="1">
+        <f t="shared" ref="N8:N35" si="2">M8*I8</f>
         <v>226.6</v>
       </c>
-      <c r="N8" s="1">
+      <c r="O8" s="1">
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
@@ -1137,33 +1167,34 @@
       <c r="F9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="1">
+      <c r="G9" s="16"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="1">
         <v>0.47699999999999998</v>
       </c>
-      <c r="I9" s="1">
+      <c r="J9" s="1">
         <v>1</v>
       </c>
-      <c r="J9" s="1">
-        <f t="shared" ref="J9:J47" si="3">H9*I9</f>
+      <c r="K9" s="1">
+        <f t="shared" ref="K9:K47" si="3">I9*J9</f>
         <v>0.47699999999999998</v>
       </c>
-      <c r="K9" s="1">
-        <v>0</v>
-      </c>
       <c r="L9" s="1">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="M9" s="1">
+      <c r="N9" s="1">
         <f t="shared" si="2"/>
         <v>52.47</v>
       </c>
-      <c r="N9" s="1">
+      <c r="O9" s="1">
         <v>110</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>76</v>
       </c>
@@ -1182,33 +1213,36 @@
       <c r="F10" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="7"/>
-      <c r="H10" s="1">
+      <c r="G10" s="16">
+        <v>1</v>
+      </c>
+      <c r="H10" s="7"/>
+      <c r="I10" s="1">
         <v>0.18</v>
       </c>
-      <c r="I10" s="1">
+      <c r="J10" s="1">
         <v>1</v>
       </c>
-      <c r="J10" s="1">
+      <c r="K10" s="1">
         <f t="shared" si="3"/>
         <v>0.18</v>
       </c>
-      <c r="K10" s="1">
+      <c r="L10" s="1">
         <v>100</v>
       </c>
-      <c r="L10" s="1">
+      <c r="M10" s="1">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="M10" s="1">
+      <c r="N10" s="1">
         <f t="shared" si="2"/>
         <v>1.7999999999999998</v>
       </c>
-      <c r="N10" s="1">
+      <c r="O10" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>74</v>
       </c>
@@ -1227,33 +1261,34 @@
       <c r="F11" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="1">
+      <c r="G11" s="15"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="1">
         <v>6</v>
       </c>
-      <c r="I11" s="1">
+      <c r="J11" s="1">
         <v>1</v>
       </c>
-      <c r="J11" s="1">
+      <c r="K11" s="1">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="K11" s="1">
-        <v>0</v>
-      </c>
       <c r="L11" s="1">
+        <v>0</v>
+      </c>
+      <c r="M11" s="1">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="M11" s="1">
+      <c r="N11" s="1">
         <f t="shared" si="2"/>
         <v>660</v>
       </c>
-      <c r="N11" s="1">
+      <c r="O11" s="1">
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>75</v>
       </c>
@@ -1272,33 +1307,36 @@
       <c r="F12" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="1">
+      <c r="G12" s="16">
+        <v>1</v>
+      </c>
+      <c r="H12" s="7"/>
+      <c r="I12" s="1">
         <v>2.11</v>
       </c>
-      <c r="I12" s="1">
+      <c r="J12" s="1">
         <v>1</v>
       </c>
-      <c r="J12" s="1">
+      <c r="K12" s="1">
         <f t="shared" si="3"/>
         <v>2.11</v>
       </c>
-      <c r="K12" s="1">
-        <v>0</v>
-      </c>
       <c r="L12" s="1">
+        <v>0</v>
+      </c>
+      <c r="M12" s="1">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="M12" s="1">
+      <c r="N12" s="1">
         <f t="shared" si="2"/>
         <v>232.1</v>
       </c>
-      <c r="N12" s="1">
+      <c r="O12" s="1">
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>77</v>
       </c>
@@ -1317,33 +1355,36 @@
       <c r="F13" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="1">
+      <c r="G13" s="15">
+        <v>1</v>
+      </c>
+      <c r="H13" s="7"/>
+      <c r="I13" s="1">
         <v>1.03</v>
       </c>
-      <c r="I13" s="1">
+      <c r="J13" s="1">
         <v>1</v>
       </c>
-      <c r="J13" s="1">
+      <c r="K13" s="1">
         <f t="shared" si="3"/>
         <v>1.03</v>
       </c>
-      <c r="K13" s="1">
-        <v>0</v>
-      </c>
       <c r="L13" s="1">
+        <v>0</v>
+      </c>
+      <c r="M13" s="1">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="M13" s="1">
+      <c r="N13" s="1">
         <f t="shared" si="2"/>
         <v>113.3</v>
       </c>
-      <c r="N13" s="1">
+      <c r="O13" s="1">
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>46</v>
       </c>
@@ -1356,30 +1397,31 @@
       <c r="D14" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G14" s="7"/>
-      <c r="H14" s="1">
+      <c r="G14" s="15"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="1">
         <v>0.08</v>
       </c>
-      <c r="I14" s="1">
+      <c r="J14" s="1">
         <v>1</v>
       </c>
-      <c r="J14" s="1">
+      <c r="K14" s="1">
         <f t="shared" si="3"/>
         <v>0.08</v>
       </c>
-      <c r="K14" s="1">
+      <c r="L14" s="1">
         <v>110</v>
       </c>
-      <c r="L14" s="1">
+      <c r="M14" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M14" s="1">
+      <c r="N14" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>84</v>
       </c>
@@ -1392,30 +1434,31 @@
       <c r="D15" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="G15" s="7"/>
-      <c r="H15" s="1">
+      <c r="G15" s="15"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="1">
         <v>0.05</v>
       </c>
-      <c r="I15" s="1">
+      <c r="J15" s="1">
         <v>10</v>
       </c>
-      <c r="J15" s="1">
+      <c r="K15" s="1">
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K15" s="1">
+      <c r="L15" s="1">
         <v>1500</v>
       </c>
-      <c r="L15" s="1">
+      <c r="M15" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M15" s="1">
+      <c r="N15" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>32</v>
       </c>
@@ -1425,30 +1468,31 @@
       <c r="D16" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="G16" s="7"/>
-      <c r="H16" s="1">
+      <c r="G16" s="15"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="1">
         <v>0.6</v>
       </c>
-      <c r="I16" s="1">
+      <c r="J16" s="1">
         <v>1</v>
       </c>
-      <c r="J16" s="1">
+      <c r="K16" s="1">
         <f t="shared" si="3"/>
         <v>0.6</v>
       </c>
-      <c r="K16" s="1">
+      <c r="L16" s="1">
         <v>110</v>
       </c>
-      <c r="L16" s="1">
+      <c r="M16" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M16" s="1">
+      <c r="N16" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>10</v>
       </c>
@@ -1458,30 +1502,31 @@
       <c r="D17" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="G17" s="7"/>
-      <c r="H17" s="1">
+      <c r="G17" s="15"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="1">
         <v>1.85</v>
       </c>
-      <c r="I17" s="1">
+      <c r="J17" s="1">
         <v>1</v>
       </c>
-      <c r="J17" s="1">
+      <c r="K17" s="1">
         <f t="shared" si="3"/>
         <v>1.85</v>
       </c>
-      <c r="K17" s="1">
+      <c r="L17" s="1">
         <v>110</v>
       </c>
-      <c r="L17" s="1">
+      <c r="M17" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M17" s="1">
+      <c r="N17" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>114</v>
       </c>
@@ -1497,35 +1542,38 @@
       <c r="F18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="G18" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="H18" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="H18" s="1">
+      <c r="I18" s="1">
         <v>0.127</v>
       </c>
-      <c r="I18" s="1">
+      <c r="J18" s="1">
         <v>16</v>
       </c>
-      <c r="J18" s="1">
+      <c r="K18" s="1">
         <f t="shared" si="3"/>
         <v>2.032</v>
       </c>
-      <c r="K18" s="1">
-        <v>0</v>
-      </c>
       <c r="L18" s="1">
+        <v>0</v>
+      </c>
+      <c r="M18" s="1">
         <f t="shared" si="1"/>
         <v>1760</v>
       </c>
-      <c r="M18" s="1">
+      <c r="N18" s="1">
         <f t="shared" si="2"/>
         <v>223.52</v>
       </c>
-      <c r="N18" s="1">
+      <c r="O18" s="1">
         <v>2500</v>
       </c>
     </row>
-    <row r="19" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>42</v>
       </c>
@@ -1541,32 +1589,35 @@
       <c r="F19" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="G19" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="H19" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="H19" s="1">
+      <c r="I19" s="1">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="I19" s="1">
+      <c r="J19" s="1">
         <v>4</v>
       </c>
-      <c r="J19" s="1">
+      <c r="K19" s="1">
         <f t="shared" si="3"/>
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="K19" s="1">
+      <c r="L19" s="1">
         <v>1000</v>
       </c>
-      <c r="L19" s="1">
+      <c r="M19" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M19" s="1">
+      <c r="N19" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>43</v>
       </c>
@@ -1582,35 +1633,38 @@
       <c r="F20" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="G20" s="15">
+        <v>1.45</v>
+      </c>
+      <c r="H20" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="H20" s="1">
+      <c r="I20" s="1">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="I20" s="1">
+      <c r="J20" s="1">
         <v>1</v>
       </c>
-      <c r="J20" s="1">
+      <c r="K20" s="1">
         <f t="shared" si="3"/>
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="K20" s="1">
-        <v>0</v>
-      </c>
       <c r="L20" s="1">
+        <v>0</v>
+      </c>
+      <c r="M20" s="1">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="M20" s="1">
+      <c r="N20" s="1">
         <f t="shared" si="2"/>
         <v>3.74</v>
       </c>
-      <c r="N20" s="1">
+      <c r="O20" s="1">
         <v>125</v>
       </c>
     </row>
-    <row r="21" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>44</v>
       </c>
@@ -1626,35 +1680,38 @@
       <c r="F21" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="G21" s="7" t="s">
+      <c r="G21" s="15">
+        <v>1.45</v>
+      </c>
+      <c r="H21" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="H21" s="1">
+      <c r="I21" s="1">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="I21" s="1">
+      <c r="J21" s="1">
         <v>1</v>
       </c>
-      <c r="J21" s="1">
+      <c r="K21" s="1">
         <f t="shared" si="3"/>
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="K21" s="1">
-        <v>0</v>
-      </c>
       <c r="L21" s="1">
+        <v>0</v>
+      </c>
+      <c r="M21" s="1">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="M21" s="1">
+      <c r="N21" s="1">
         <f t="shared" si="2"/>
         <v>3.8500000000000005</v>
       </c>
-      <c r="N21" s="1">
+      <c r="O21" s="1">
         <v>125</v>
       </c>
     </row>
-    <row r="22" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>127</v>
       </c>
@@ -1670,35 +1727,38 @@
       <c r="F22" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="G22" s="15">
+        <v>1.45</v>
+      </c>
+      <c r="H22" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="H22" s="1">
+      <c r="I22" s="1">
         <v>3.1E-2</v>
       </c>
-      <c r="I22" s="1">
+      <c r="J22" s="1">
         <v>1</v>
       </c>
-      <c r="J22" s="1">
+      <c r="K22" s="1">
         <f t="shared" si="3"/>
         <v>3.1E-2</v>
       </c>
-      <c r="K22" s="1">
-        <v>0</v>
-      </c>
       <c r="L22" s="1">
+        <v>0</v>
+      </c>
+      <c r="M22" s="1">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="M22" s="1">
+      <c r="N22" s="1">
         <f t="shared" si="2"/>
         <v>3.41</v>
       </c>
-      <c r="N22" s="1">
+      <c r="O22" s="1">
         <v>125</v>
       </c>
     </row>
-    <row r="23" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>49</v>
       </c>
@@ -1714,35 +1774,36 @@
       <c r="F23" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="G23" s="7" t="s">
+      <c r="G23" s="15"/>
+      <c r="H23" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="H23" s="1">
+      <c r="I23" s="1">
         <v>0.16700000000000001</v>
       </c>
-      <c r="I23" s="1">
+      <c r="J23" s="1">
         <v>1</v>
       </c>
-      <c r="J23" s="1">
+      <c r="K23" s="1">
         <f t="shared" si="3"/>
         <v>0.16700000000000001</v>
       </c>
-      <c r="K23" s="1">
-        <v>0</v>
-      </c>
       <c r="L23" s="1">
+        <v>0</v>
+      </c>
+      <c r="M23" s="1">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="M23" s="1">
+      <c r="N23" s="1">
         <f t="shared" si="2"/>
         <v>18.37</v>
       </c>
-      <c r="N23" s="1">
+      <c r="O23" s="1">
         <v>125</v>
       </c>
     </row>
-    <row r="24" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>51</v>
       </c>
@@ -1758,35 +1819,38 @@
       <c r="F24" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="G24" s="7" t="s">
+      <c r="G24" s="15">
+        <v>1</v>
+      </c>
+      <c r="H24" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="H24" s="1">
+      <c r="I24" s="1">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="I24" s="1">
+      <c r="J24" s="1">
         <v>1</v>
       </c>
-      <c r="J24" s="1">
+      <c r="K24" s="1">
         <f t="shared" si="3"/>
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="K24" s="1">
+      <c r="L24" s="1">
         <v>100</v>
       </c>
-      <c r="L24" s="1">
+      <c r="M24" s="1">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="M24" s="1">
+      <c r="N24" s="1">
         <f t="shared" si="2"/>
         <v>0.48</v>
       </c>
-      <c r="N24" s="1">
+      <c r="O24" s="1">
         <v>125</v>
       </c>
     </row>
-    <row r="25" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>54</v>
       </c>
@@ -1802,32 +1866,35 @@
       <c r="F25" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="G25" s="7" t="s">
+      <c r="G25" s="16">
+        <v>0.45</v>
+      </c>
+      <c r="H25" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="H25" s="1">
+      <c r="I25" s="1">
         <v>1E-3</v>
       </c>
-      <c r="I25" s="1">
+      <c r="J25" s="1">
         <v>2</v>
       </c>
-      <c r="J25" s="1">
+      <c r="K25" s="1">
         <f t="shared" si="3"/>
         <v>2E-3</v>
       </c>
-      <c r="K25" s="1">
+      <c r="L25" s="1">
         <v>5000</v>
       </c>
-      <c r="L25" s="1">
+      <c r="M25" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M25" s="1">
+      <c r="N25" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>56</v>
       </c>
@@ -1843,32 +1910,35 @@
       <c r="F26" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="G26" s="7" t="s">
+      <c r="G26" s="16">
+        <v>0.45</v>
+      </c>
+      <c r="H26" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="H26" s="1">
+      <c r="I26" s="1">
         <v>1E-3</v>
       </c>
-      <c r="I26" s="1">
+      <c r="J26" s="1">
         <v>1</v>
       </c>
-      <c r="J26" s="1">
+      <c r="K26" s="1">
         <f t="shared" si="3"/>
         <v>1E-3</v>
       </c>
-      <c r="K26" s="1">
+      <c r="L26" s="1">
         <v>5000</v>
       </c>
-      <c r="L26" s="1">
+      <c r="M26" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M26" s="1">
+      <c r="N26" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>58</v>
       </c>
@@ -1884,32 +1954,35 @@
       <c r="F27" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="G27" s="7" t="s">
+      <c r="G27" s="16">
+        <v>0.45</v>
+      </c>
+      <c r="H27" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="H27" s="1">
+      <c r="I27" s="1">
         <v>1E-3</v>
       </c>
-      <c r="I27" s="1">
+      <c r="J27" s="1">
         <v>3</v>
       </c>
-      <c r="J27" s="1">
+      <c r="K27" s="1">
         <f t="shared" si="3"/>
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="K27" s="1">
+      <c r="L27" s="1">
         <v>5000</v>
       </c>
-      <c r="L27" s="1">
+      <c r="M27" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M27" s="1">
+      <c r="N27" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>60</v>
       </c>
@@ -1925,32 +1998,35 @@
       <c r="F28" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="G28" s="7" t="s">
+      <c r="G28" s="16">
+        <v>0.45</v>
+      </c>
+      <c r="H28" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="H28" s="1">
+      <c r="I28" s="1">
         <v>1E-3</v>
       </c>
-      <c r="I28" s="1">
+      <c r="J28" s="1">
         <v>1</v>
       </c>
-      <c r="J28" s="1">
+      <c r="K28" s="1">
         <f t="shared" si="3"/>
         <v>1E-3</v>
       </c>
-      <c r="K28" s="1">
+      <c r="L28" s="1">
         <v>5000</v>
       </c>
-      <c r="L28" s="1">
+      <c r="M28" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M28" s="1">
+      <c r="N28" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>62</v>
       </c>
@@ -1966,32 +2042,35 @@
       <c r="F29" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="G29" s="7" t="s">
+      <c r="G29" s="16">
+        <v>0.45</v>
+      </c>
+      <c r="H29" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="H29" s="1">
+      <c r="I29" s="1">
         <v>1E-3</v>
       </c>
-      <c r="I29" s="1">
+      <c r="J29" s="1">
         <v>1</v>
       </c>
-      <c r="J29" s="1">
+      <c r="K29" s="1">
         <f t="shared" si="3"/>
         <v>1E-3</v>
       </c>
-      <c r="K29" s="1">
+      <c r="L29" s="1">
         <v>5000</v>
       </c>
-      <c r="L29" s="1">
+      <c r="M29" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M29" s="1">
+      <c r="N29" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>64</v>
       </c>
@@ -2007,35 +2086,38 @@
       <c r="F30" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="G30" s="7" t="s">
+      <c r="G30" s="16">
+        <v>0.45</v>
+      </c>
+      <c r="H30" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="H30" s="1">
+      <c r="I30" s="1">
         <v>1E-3</v>
       </c>
-      <c r="I30" s="1">
+      <c r="J30" s="1">
         <v>1</v>
       </c>
-      <c r="J30" s="1">
+      <c r="K30" s="1">
         <f t="shared" si="3"/>
         <v>1E-3</v>
       </c>
-      <c r="K30" s="1">
-        <v>0</v>
-      </c>
       <c r="L30" s="1">
+        <v>0</v>
+      </c>
+      <c r="M30" s="1">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="M30" s="1">
+      <c r="N30" s="1">
         <f t="shared" si="2"/>
         <v>0.11</v>
       </c>
-      <c r="N30" s="1">
+      <c r="O30" s="1">
         <v>5000</v>
       </c>
     </row>
-    <row r="31" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>66</v>
       </c>
@@ -2051,35 +2133,38 @@
       <c r="F31" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="G31" s="7" t="s">
+      <c r="G31" s="16">
+        <v>0.45</v>
+      </c>
+      <c r="H31" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="H31" s="1">
+      <c r="I31" s="1">
         <v>1E-3</v>
       </c>
-      <c r="I31" s="1">
+      <c r="J31" s="1">
         <v>1</v>
       </c>
-      <c r="J31" s="1">
+      <c r="K31" s="1">
         <f t="shared" si="3"/>
         <v>1E-3</v>
       </c>
-      <c r="K31" s="1">
-        <v>0</v>
-      </c>
       <c r="L31" s="1">
+        <v>0</v>
+      </c>
+      <c r="M31" s="1">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="M31" s="1">
+      <c r="N31" s="1">
         <f t="shared" si="2"/>
         <v>0.11</v>
       </c>
-      <c r="N31" s="1">
+      <c r="O31" s="1">
         <v>5000</v>
       </c>
     </row>
-    <row r="32" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>68</v>
       </c>
@@ -2087,32 +2172,35 @@
         <v>69</v>
       </c>
       <c r="D32" s="7"/>
-      <c r="G32" s="7" t="s">
+      <c r="G32" s="16">
+        <v>0.45</v>
+      </c>
+      <c r="H32" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="H32" s="1">
+      <c r="I32" s="1">
         <v>1E-3</v>
       </c>
-      <c r="I32" s="1">
+      <c r="J32" s="1">
         <v>1</v>
       </c>
-      <c r="J32" s="1">
+      <c r="K32" s="1">
         <f t="shared" si="3"/>
         <v>1E-3</v>
       </c>
-      <c r="K32" s="1">
+      <c r="L32" s="1">
         <v>5000</v>
       </c>
-      <c r="L32" s="1">
+      <c r="M32" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M32" s="1">
+      <c r="N32" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>70</v>
       </c>
@@ -2120,30 +2208,31 @@
         <v>71</v>
       </c>
       <c r="D33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="1">
+      <c r="G33" s="15"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="1">
         <v>0.27</v>
       </c>
-      <c r="I33" s="1">
+      <c r="J33" s="1">
         <v>10</v>
       </c>
-      <c r="J33" s="1">
+      <c r="K33" s="1">
         <f t="shared" si="3"/>
         <v>2.7</v>
       </c>
-      <c r="K33" s="1">
+      <c r="L33" s="1">
         <v>1300</v>
       </c>
-      <c r="L33" s="1">
+      <c r="M33" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M33" s="1">
+      <c r="N33" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>72</v>
       </c>
@@ -2159,33 +2248,34 @@
       <c r="F34" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="G34" s="7"/>
-      <c r="H34" s="1">
+      <c r="G34" s="15"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="1">
         <v>1.1000000000000001</v>
       </c>
-      <c r="I34" s="1">
+      <c r="J34" s="1">
         <v>2</v>
       </c>
-      <c r="J34" s="1">
+      <c r="K34" s="1">
         <f t="shared" si="3"/>
         <v>2.2000000000000002</v>
       </c>
-      <c r="K34" s="1">
-        <v>0</v>
-      </c>
       <c r="L34" s="1">
+        <v>0</v>
+      </c>
+      <c r="M34" s="1">
         <f t="shared" si="1"/>
         <v>220</v>
       </c>
-      <c r="M34" s="1">
+      <c r="N34" s="1">
         <f t="shared" si="2"/>
         <v>242.00000000000003</v>
       </c>
-      <c r="N34" s="1">
+      <c r="O34" s="1">
         <v>125</v>
       </c>
     </row>
-    <row r="35" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>112</v>
       </c>
@@ -2201,52 +2291,55 @@
       <c r="F35" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="G35" s="7"/>
-      <c r="H35" s="1">
+      <c r="G35" s="15"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="1">
         <v>0.53400000000000003</v>
       </c>
-      <c r="I35" s="1">
+      <c r="J35" s="1">
         <v>1</v>
       </c>
-      <c r="J35" s="1">
+      <c r="K35" s="1">
         <f t="shared" si="3"/>
         <v>0.53400000000000003</v>
       </c>
-      <c r="K35" s="1">
-        <v>0</v>
-      </c>
       <c r="L35" s="1">
+        <v>0</v>
+      </c>
+      <c r="M35" s="1">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="M35" s="1">
+      <c r="N35" s="1">
         <f t="shared" si="2"/>
         <v>58.74</v>
       </c>
-      <c r="N35" s="1">
+      <c r="O35" s="1">
         <v>125</v>
       </c>
     </row>
-    <row r="36" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="J36" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="G36" s="15"/>
+      <c r="H36" s="7"/>
+      <c r="K36" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>105</v>
       </c>
       <c r="D37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="J37" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="G37" s="15"/>
+      <c r="H37" s="7"/>
+      <c r="K37" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="1" t="s">
         <v>106</v>
@@ -2255,19 +2348,20 @@
         <v>139</v>
       </c>
       <c r="D38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="1">
-        <v>1</v>
-      </c>
+      <c r="G38" s="15"/>
+      <c r="H38" s="7"/>
       <c r="I38" s="1">
         <v>1</v>
       </c>
       <c r="J38" s="1">
-        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="K38" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="1" t="s">
         <v>107</v>
@@ -2276,19 +2370,20 @@
         <v>140</v>
       </c>
       <c r="D39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="1">
+      <c r="G39" s="15"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="1">
         <v>2</v>
       </c>
-      <c r="I39" s="1">
+      <c r="J39" s="1">
         <v>1</v>
       </c>
-      <c r="J39" s="1">
+      <c r="K39" s="1">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="1" t="s">
         <v>108</v>
@@ -2297,19 +2392,20 @@
         <v>141</v>
       </c>
       <c r="D40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="1">
+      <c r="G40" s="15"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="1">
         <v>0.31</v>
       </c>
-      <c r="I40" s="1">
+      <c r="J40" s="1">
         <v>3</v>
       </c>
-      <c r="J40" s="1">
+      <c r="K40" s="1">
         <f t="shared" si="3"/>
         <v>0.92999999999999994</v>
       </c>
     </row>
-    <row r="41" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="1" t="s">
         <v>109</v>
@@ -2318,19 +2414,20 @@
         <v>141</v>
       </c>
       <c r="D41" s="7"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="1">
+      <c r="G41" s="15"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="1">
         <v>0.45</v>
       </c>
-      <c r="I41" s="1">
+      <c r="J41" s="1">
         <v>1</v>
       </c>
-      <c r="J41" s="1">
+      <c r="K41" s="1">
         <f t="shared" si="3"/>
         <v>0.45</v>
       </c>
     </row>
-    <row r="42" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="1" t="s">
         <v>110</v>
@@ -2339,19 +2436,20 @@
         <v>141</v>
       </c>
       <c r="D42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="1">
+      <c r="G42" s="15"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="1">
         <v>0.5</v>
       </c>
-      <c r="I42" s="1">
+      <c r="J42" s="1">
         <v>2</v>
       </c>
-      <c r="J42" s="1">
+      <c r="K42" s="1">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="1" t="s">
         <v>111</v>
@@ -2360,19 +2458,20 @@
         <v>141</v>
       </c>
       <c r="D43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="1">
+      <c r="G43" s="15"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="1">
         <v>0.25</v>
       </c>
-      <c r="I43" s="1">
+      <c r="J43" s="1">
         <v>10</v>
       </c>
-      <c r="J43" s="1">
+      <c r="K43" s="1">
         <f t="shared" si="3"/>
         <v>2.5</v>
       </c>
     </row>
-    <row r="44" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="1" t="s">
         <v>118</v>
@@ -2381,19 +2480,20 @@
         <v>141</v>
       </c>
       <c r="D44" s="7"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="1">
+      <c r="G44" s="15"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="1">
         <v>4</v>
       </c>
-      <c r="I44" s="1">
+      <c r="J44" s="1">
         <v>2</v>
       </c>
-      <c r="J44" s="1">
+      <c r="K44" s="1">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="1" t="s">
         <v>119</v>
@@ -2402,19 +2502,20 @@
         <v>142</v>
       </c>
       <c r="D45" s="7"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="1">
+      <c r="G45" s="15"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="1">
         <v>8</v>
       </c>
-      <c r="I45" s="1">
+      <c r="J45" s="1">
         <v>0.1</v>
       </c>
-      <c r="J45" s="1">
+      <c r="K45" s="1">
         <f t="shared" si="3"/>
         <v>0.8</v>
       </c>
     </row>
-    <row r="46" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="1" t="s">
         <v>120</v>
@@ -2423,80 +2524,84 @@
         <v>142</v>
       </c>
       <c r="D46" s="7"/>
-      <c r="G46" s="7"/>
-      <c r="H46" s="1">
+      <c r="G46" s="15"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="1">
         <v>0.25</v>
       </c>
-      <c r="I46" s="1">
+      <c r="J46" s="1">
         <v>1</v>
       </c>
-      <c r="J46" s="1">
+      <c r="K46" s="1">
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
     </row>
-    <row r="47" spans="1:14" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D47" s="7"/>
-      <c r="G47" s="7"/>
-      <c r="J47" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="G47" s="15"/>
+      <c r="H47" s="7"/>
+      <c r="K47" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="D48" s="8"/>
-      <c r="G48" s="8"/>
-    </row>
-    <row r="49" spans="2:8" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="G48" s="17"/>
+      <c r="H48" s="8"/>
+    </row>
+    <row r="49" spans="2:9" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
         <v>143</v>
       </c>
       <c r="D49" s="7"/>
-      <c r="G49" s="7"/>
-    </row>
-    <row r="50" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="G49" s="15"/>
+      <c r="H49" s="7"/>
+    </row>
+    <row r="50" spans="2:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
         <v>144</v>
       </c>
       <c r="C50">
         <v>2500</v>
       </c>
-      <c r="G50" s="9" t="s">
+      <c r="H50" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="H50">
-        <f>SUM(J2:J49)</f>
+      <c r="I50">
+        <f>SUM(K2:K49)</f>
         <v>52.189800000000005</v>
       </c>
     </row>
-    <row r="51" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
         <v>154</v>
       </c>
       <c r="C51">
         <v>1100</v>
       </c>
-      <c r="G51" s="6" t="s">
+      <c r="H51" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="H51">
-        <f>SUM(M7:M35)</f>
+      <c r="I51">
+        <f>SUM(N7:N35)</f>
         <v>2679.5479999999993</v>
       </c>
     </row>
-    <row r="52" spans="2:8" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="2:8" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="2:8" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="2:8" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="2:8" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="2:8" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="2:8" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="2:8" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="2:8" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="2:8" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="2:8" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="2:8" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="2:8" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="2:9" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="2:9" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="2:9" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="2:9" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="2:9" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="2:9" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="2:9" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="2:9" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="2:9" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="2:9" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="2:9" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="2:9" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="2:9" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="65" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="66" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="67" ht="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>